<commit_message>
Listed all part names and designators
</commit_message>
<xml_diff>
--- a/Hardware/MoodBadge-BOM.xlsx
+++ b/Hardware/MoodBadge-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orlandohoilett/Documents/Milestones/Git/Tasks-Tutorials-Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan Singer\mood-badge\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6F0319-899B-F545-ABC0-B856698FB7B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35106581-CBBA-42C2-9F5F-056EDEF528E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="130">
   <si>
     <t>BOM #</t>
   </si>
@@ -602,7 +602,223 @@
     <t>RMCF0603FT10K0CT-ND</t>
   </si>
   <si>
-    <t>Design Name -- Revision Code / Designer or Organization Name</t>
+    <t>Mood Badge -- V1 / Megan Singer</t>
+  </si>
+  <si>
+    <t>BOOT</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>CHRG</t>
+  </si>
+  <si>
+    <t>MCP73831</t>
+  </si>
+  <si>
+    <t>SOT23-5</t>
+  </si>
+  <si>
+    <t>SPST.KT11P4SM34LFS</t>
+  </si>
+  <si>
+    <t>FTDI_DEVICE</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>PCF8574T</t>
+  </si>
+  <si>
+    <t>SO16W</t>
+  </si>
+  <si>
+    <t>LED8</t>
+  </si>
+  <si>
+    <t>LIPO</t>
+  </si>
+  <si>
+    <t>SEGMENT_8X8_ROWCATHODEBL-M12A883</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>SPST-PTS830GG140</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>USB1</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>MATRIX</t>
+  </si>
+  <si>
+    <t>ON/OFF</t>
+  </si>
+  <si>
+    <t>SWITCH.JS202011JXQNUPWARDS</t>
+  </si>
+  <si>
+    <t>100 nF capacitor</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C5, C6, C7, C15, C21</t>
+  </si>
+  <si>
+    <t>4.7 uF capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C8, C9, C16, C17, C18, </t>
+  </si>
+  <si>
+    <t>2.2 uF capacitor</t>
+  </si>
+  <si>
+    <t>C10, C19</t>
+  </si>
+  <si>
+    <t>1 uF capacitor</t>
+  </si>
+  <si>
+    <t>0.1 uF capacitor</t>
+  </si>
+  <si>
+    <t>C11, C14</t>
+  </si>
+  <si>
+    <t>22 pF capacitor</t>
+  </si>
+  <si>
+    <t>C12, C13</t>
+  </si>
+  <si>
+    <t>205 ohm resistor</t>
+  </si>
+  <si>
+    <t>R16, R17, R18, R19, R20, R21, R22, R23</t>
+  </si>
+  <si>
+    <t>487 ohm resistor</t>
+  </si>
+  <si>
+    <t>1 kohm resistor</t>
+  </si>
+  <si>
+    <t>R2, R4, R6, R8, R10, R12, R13</t>
+  </si>
+  <si>
+    <t>10 kohm resistor</t>
+  </si>
+  <si>
+    <t>R1, R3, R5, R7, R9, R11, R14, R15, R26</t>
+  </si>
+  <si>
+    <t>12 kohm resistor</t>
+  </si>
+  <si>
+    <t>210 kohm resistor</t>
+  </si>
+  <si>
+    <t>R28, R29</t>
+  </si>
+  <si>
+    <t>3.3 Mohm resistor</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>UP, DOWN, LEFT, RIGHT, SELECT, MODE</t>
+  </si>
+  <si>
+    <t>LED matrix</t>
+  </si>
+  <si>
+    <t>Adafruit Industries</t>
+  </si>
+  <si>
+    <t>Large push button</t>
+  </si>
+  <si>
+    <t>Small push button</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>D1, D2, D3</t>
+  </si>
+  <si>
+    <t>Bootloader 2x3 pins</t>
+  </si>
+  <si>
+    <t>FTDI 1x6 pins</t>
+  </si>
+  <si>
+    <t>USB port</t>
+  </si>
+  <si>
+    <t>LIPO battery port</t>
+  </si>
+  <si>
+    <t>Clock crystal</t>
+  </si>
+  <si>
+    <t>CA-310</t>
+  </si>
+  <si>
+    <t>Battery charger IC</t>
+  </si>
+  <si>
+    <t>Port expander</t>
+  </si>
+  <si>
+    <t>Arduino ATMEGA328</t>
+  </si>
+  <si>
+    <t>QFP</t>
+  </si>
+  <si>
+    <t>Op amp</t>
+  </si>
+  <si>
+    <t>Transducer</t>
+  </si>
+  <si>
+    <t>APDS9008</t>
+  </si>
+  <si>
+    <t>IR LED</t>
+  </si>
+  <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7</t>
   </si>
 </sst>
 </file>
@@ -633,13 +849,6 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -686,6 +895,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -856,42 +1071,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1314,405 +1528,817 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="14.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.796875" style="1"/>
+    <col min="12" max="12" width="6.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="6">
-        <f>SUM(M3:M77)</f>
+      <c r="M1" s="5">
+        <f>SUM(M3:M81)</f>
         <v>2.48</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="6">
-        <f>SUM(O3:O77)</f>
+      <c r="O1" s="5">
+        <f>SUM(O3:O81)</f>
         <v>1.1271</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="9">
         <v>0.38</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>1</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="9">
         <f t="shared" ref="M3:M8" si="0">K3*L3</f>
         <v>0.38</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <v>0.1391</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="9">
         <f t="shared" ref="O3:O7" si="1">L3*N3</f>
         <v>0.1391</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>0.89</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <v>1</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <f t="shared" si="0"/>
         <v>0.89</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <v>0.46</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <f t="shared" si="1"/>
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="9" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="9">
         <v>0.55000000000000004</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <v>1</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="N5" s="10">
+      <c r="N5" s="9">
         <v>0.3982</v>
       </c>
-      <c r="O5" s="10">
+      <c r="O5" s="9">
         <f t="shared" si="1"/>
         <v>0.3982</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="9">
         <v>0.26</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <v>1</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="9">
         <v>9.0899999999999995E-2</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <f t="shared" si="1"/>
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="E7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="9">
         <v>0.1</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="10">
         <v>3</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="N7" s="10">
+      <c r="N7" s="9">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <f t="shared" si="1"/>
         <v>2.0399999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <v>0.1</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="10">
         <v>1</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="9">
         <v>1.8499999999999999E-2</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <f>L8*N8</f>
         <v>1.8499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="H23" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Completed a majority of the BOM. Missing 5 components
</commit_message>
<xml_diff>
--- a/Hardware/MoodBadge-BOM.xlsx
+++ b/Hardware/MoodBadge-BOM.xlsx
@@ -5,18 +5,27 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megan Singer\mood-badge\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msing\mood-badge\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35106581-CBBA-42C2-9F5F-056EDEF528E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FB91F2-588A-4064-8A2F-DAB27A155E2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -429,7 +438,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="209">
   <si>
     <t>BOM #</t>
   </si>
@@ -620,9 +629,6 @@
     <t>SOT23-5</t>
   </si>
   <si>
-    <t>SPST.KT11P4SM34LFS</t>
-  </si>
-  <si>
     <t>FTDI_DEVICE</t>
   </si>
   <si>
@@ -641,9 +647,6 @@
     <t>LIPO</t>
   </si>
   <si>
-    <t>SEGMENT_8X8_ROWCATHODEBL-M12A883</t>
-  </si>
-  <si>
     <t>OP</t>
   </si>
   <si>
@@ -662,9 +665,6 @@
     <t>RESET</t>
   </si>
   <si>
-    <t>SPST-PTS830GG140</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -680,9 +680,6 @@
     <t>ON/OFF</t>
   </si>
   <si>
-    <t>SWITCH.JS202011JXQNUPWARDS</t>
-  </si>
-  <si>
     <t>100 nF capacitor</t>
   </si>
   <si>
@@ -758,9 +755,6 @@
     <t>LED matrix</t>
   </si>
   <si>
-    <t>Adafruit Industries</t>
-  </si>
-  <si>
     <t>Large push button</t>
   </si>
   <si>
@@ -791,9 +785,6 @@
     <t>Clock crystal</t>
   </si>
   <si>
-    <t>CA-310</t>
-  </si>
-  <si>
     <t>Battery charger IC</t>
   </si>
   <si>
@@ -819,6 +810,261 @@
   </si>
   <si>
     <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>CL10B102KB8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1018-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 6.3V X5R 0603</t>
+  </si>
+  <si>
+    <t>CL10A475KQ8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1045-1-ND</t>
+  </si>
+  <si>
+    <t>1276-1183-1-ND</t>
+  </si>
+  <si>
+    <t>CL10A225KQ8NNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 2.2UF 6.3V X5R 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 25V X5R 0603</t>
+  </si>
+  <si>
+    <t>1276-1006-1-ND</t>
+  </si>
+  <si>
+    <t>CL10B104KA8NNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 22PF 50V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>1276-2228-1-ND</t>
+  </si>
+  <si>
+    <t>CL10C220JB8NFNC</t>
+  </si>
+  <si>
+    <t>738-RMCF0603FT205RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT205R</t>
+  </si>
+  <si>
+    <t>RES 205 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT487RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT487R</t>
+  </si>
+  <si>
+    <t>RES 487 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603JJ1K00CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JJ1K00</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD10K0CT-ND</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD10K0</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603JT12K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT12K0</t>
+  </si>
+  <si>
+    <t>RES 12K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT210KCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT210K</t>
+  </si>
+  <si>
+    <t>RES 210K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603JT3M30CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT3M30</t>
+  </si>
+  <si>
+    <t>RES 3.3M OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>2151-AS-16.000-20-EXT-ND</t>
+  </si>
+  <si>
+    <t>AS-16.000-20-EXT</t>
+  </si>
+  <si>
+    <t>Raltron Electronics</t>
+  </si>
+  <si>
+    <t>HC-49/US</t>
+  </si>
+  <si>
+    <t>CRYSTAL 16.0000MHZ 20PF TH</t>
+  </si>
+  <si>
+    <t>497-3381-1-ND</t>
+  </si>
+  <si>
+    <t>BAT20JFILM</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 23V 1A SOD323</t>
+  </si>
+  <si>
+    <t>SOD-323</t>
+  </si>
+  <si>
+    <t>VSMY2941RGX01CT-ND</t>
+  </si>
+  <si>
+    <t>VSMY2941RGX01</t>
+  </si>
+  <si>
+    <t>Vishay Semiconductor Opto Division</t>
+  </si>
+  <si>
+    <t>2-SMD, Z-Bend</t>
+  </si>
+  <si>
+    <t>EMITTER IR 940NM 70MA SMD</t>
+  </si>
+  <si>
+    <t>Lite-On Inc.</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR CHIP SMD</t>
+  </si>
+  <si>
+    <t>LTST-C191TBKT-5A</t>
+  </si>
+  <si>
+    <t>160-2212-1-ND</t>
+  </si>
+  <si>
+    <t>Adafruit Industries LLC</t>
+  </si>
+  <si>
+    <t>LED MATRIX 8X8 SQUARE GREEN</t>
+  </si>
+  <si>
+    <t>1528-2216-ND</t>
+  </si>
+  <si>
+    <t>CKN1860CT-ND</t>
+  </si>
+  <si>
+    <t>KT11P4SM34LFS</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 1VA 32V</t>
+  </si>
+  <si>
+    <t>CKN10588CT-ND</t>
+  </si>
+  <si>
+    <t>PTS830GG140 SMTR LFS</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>CKN10723CT-ND</t>
+  </si>
+  <si>
+    <t>JS202011JCQN</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 6POS 2.54MM</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE DPDT 300MA 6V</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>PREC003DAAN-RC</t>
+  </si>
+  <si>
+    <t>S2012EC-03-ND</t>
+  </si>
+  <si>
+    <t>1849-PR20206VBNN-ND</t>
+  </si>
+  <si>
+    <t>PR20206VBNN</t>
+  </si>
+  <si>
+    <t>METZ CONNECT USA Inc.</t>
+  </si>
+  <si>
+    <t>PIN HEADER, THR, SINGLE ROW, .10</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB2.0 MICRO B SMD R/A</t>
+  </si>
+  <si>
+    <t>Amphenol ICC (FCI)</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>609-4613-1-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD R/A 2POS 2MM</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>S2B-PH-SM4-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1749-1-ND</t>
   </si>
 </sst>
 </file>
@@ -829,7 +1075,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -901,6 +1147,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -987,7 +1240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="82">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1070,8 +1323,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1108,8 +1362,22 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="82" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="1" xfId="82" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="82" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="3" borderId="1" xfId="82" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="82">
+  <cellStyles count="83">
+    <cellStyle name="Currency" xfId="82" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1530,28 +1798,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="133" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="11.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.796875" style="1"/>
-    <col min="12" max="12" width="6.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.796875" style="1"/>
+    <col min="10" max="10" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="17"/>
+    <col min="12" max="12" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.83203125" style="17"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.45">
       <c r="A1" s="11" t="s">
         <v>57</v>
       </c>
@@ -1564,23 +1833,23 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="K1" s="14"/>
       <c r="L1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="18">
         <f>SUM(M3:M81)</f>
-        <v>2.48</v>
-      </c>
-      <c r="N1" s="4" t="s">
+        <v>40.739999999999995</v>
+      </c>
+      <c r="N1" s="18" t="s">
         <v>47</v>
       </c>
       <c r="O1" s="5">
         <f>SUM(O3:O81)</f>
-        <v>1.1271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>26.848480000000006</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1611,23 +1880,23 @@
       <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="15" t="s">
         <v>27</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <f>1</f>
         <v>1</v>
@@ -1659,17 +1928,17 @@
       <c r="J3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="16">
         <v>0.38</v>
       </c>
       <c r="L3" s="10">
         <v>1</v>
       </c>
-      <c r="M3" s="9">
-        <f t="shared" ref="M3:M8" si="0">K3*L3</f>
+      <c r="M3" s="16">
+        <f t="shared" ref="M3:M39" si="0">K3*L3</f>
         <v>0.38</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="16">
         <v>0.1391</v>
       </c>
       <c r="O3" s="9">
@@ -1677,7 +1946,7 @@
         <v>0.1391</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1708,17 +1977,17 @@
       <c r="J4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="16">
         <v>0.89</v>
       </c>
       <c r="L4" s="10">
         <v>1</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="16">
         <f t="shared" si="0"/>
         <v>0.89</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="16">
         <v>0.46</v>
       </c>
       <c r="O4" s="9">
@@ -1726,7 +1995,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -1755,17 +2024,17 @@
       <c r="J5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="16">
         <v>0.55000000000000004</v>
       </c>
       <c r="L5" s="10">
         <v>1</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="16">
         <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="N5" s="9">
+      <c r="N5" s="16">
         <v>0.3982</v>
       </c>
       <c r="O5" s="9">
@@ -1773,7 +2042,7 @@
         <v>0.3982</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -1804,17 +2073,17 @@
       <c r="J6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="16">
         <v>0.26</v>
       </c>
       <c r="L6" s="10">
         <v>1</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="16">
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="16">
         <v>9.0899999999999995E-2</v>
       </c>
       <c r="O6" s="9">
@@ -1822,7 +2091,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -1853,17 +2122,17 @@
       <c r="J7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="16">
         <v>0.1</v>
       </c>
       <c r="L7" s="10">
         <v>3</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="16">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="16">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O7" s="9">
@@ -1871,7 +2140,7 @@
         <v>2.0399999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -1902,17 +2171,17 @@
       <c r="J8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="16">
         <v>0.1</v>
       </c>
       <c r="L8" s="10">
         <v>1</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="16">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="16">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="O8" s="9">
@@ -1920,12 +2189,22 @@
         <v>1.8499999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M9" s="16"/>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>12</v>
@@ -1933,13 +2212,48 @@
       <c r="F10" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>8</v>
+      </c>
+      <c r="M10" s="16">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="N10" s="17">
+        <v>1.43E-2</v>
+      </c>
+      <c r="O10" s="9">
+        <f t="shared" ref="O9:O39" si="2">L10*N10</f>
+        <v>0.1144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -1947,13 +2261,48 @@
       <c r="F11" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>6</v>
+      </c>
+      <c r="M11" s="16">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="N11" s="17">
+        <v>2.01E-2</v>
+      </c>
+      <c r="O11" s="9">
+        <f t="shared" si="2"/>
+        <v>0.1206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
@@ -1961,27 +2310,97 @@
       <c r="F12" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>2</v>
+      </c>
+      <c r="M12" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N12" s="17">
+        <v>1.95E-2</v>
+      </c>
+      <c r="O12" s="9">
+        <f t="shared" si="2"/>
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="16">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="N13" s="17">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="O13" s="9">
+        <f t="shared" si="2"/>
+        <v>1.5900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>5</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
@@ -1989,13 +2408,48 @@
       <c r="F14" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L14" s="1">
+        <v>2</v>
+      </c>
+      <c r="M14" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N14" s="17">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="O14" s="9">
+        <f t="shared" si="2"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>12</v>
@@ -2003,13 +2457,48 @@
       <c r="F15" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K15" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2</v>
+      </c>
+      <c r="M15" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N15" s="17">
+        <v>2.104E-2</v>
+      </c>
+      <c r="O15" s="9">
+        <f t="shared" si="2"/>
+        <v>4.2079999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>7</v>
+      </c>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>12</v>
@@ -2017,13 +2506,48 @@
       <c r="F16" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K16" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>8</v>
+      </c>
+      <c r="M16" s="16">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="N16" s="17">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O16" s="9">
+        <f t="shared" si="2"/>
+        <v>5.4399999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>8</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
@@ -2031,13 +2555,48 @@
       <c r="F17" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K17" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+      <c r="M17" s="16">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="N17" s="17">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O17" s="9">
+        <f t="shared" si="2"/>
+        <v>6.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>9</v>
+      </c>
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
@@ -2045,13 +2604,48 @@
       <c r="F18" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K18" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>7</v>
+      </c>
+      <c r="M18" s="16">
+        <f t="shared" si="0"/>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="N18" s="17">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="O18" s="9">
+        <f t="shared" si="2"/>
+        <v>4.2700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>10</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
@@ -2059,13 +2653,48 @@
       <c r="F19" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K19" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>9</v>
+      </c>
+      <c r="M19" s="16">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="N19" s="17">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="O19" s="9">
+        <f t="shared" si="2"/>
+        <v>0.21240000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>11</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
@@ -2073,13 +2702,48 @@
       <c r="F20" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K20" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+      <c r="M20" s="16">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="N20" s="17">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="O20" s="9">
+        <f t="shared" si="2"/>
+        <v>6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>12</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>12</v>
@@ -2087,13 +2751,48 @@
       <c r="F21" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L21" s="1">
+        <v>2</v>
+      </c>
+      <c r="M21" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N21" s="17">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="O21" s="9">
+        <f t="shared" si="2"/>
+        <v>1.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>13</v>
+      </c>
       <c r="B22" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
@@ -2101,51 +2800,195 @@
       <c r="F22" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="16">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="N22" s="17">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="O22" s="9">
+        <f t="shared" si="2"/>
+        <v>6.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>14</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="H23" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K23" s="17">
+        <v>0.18</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="16">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="N23" s="17">
+        <v>0.12</v>
+      </c>
+      <c r="O23" s="9">
+        <f t="shared" si="2"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>15</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K24" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="L24" s="1">
+        <v>3</v>
+      </c>
+      <c r="M24" s="16">
+        <f t="shared" si="0"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="N24" s="17">
+        <v>0.15229999999999999</v>
+      </c>
+      <c r="O24" s="9">
+        <f t="shared" si="2"/>
+        <v>0.45689999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K25" s="17">
+        <v>0.61</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="16">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="N25" s="17">
+        <v>0.4103</v>
+      </c>
+      <c r="O25" s="9">
+        <f t="shared" si="2"/>
+        <v>0.4103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>12</v>
@@ -2153,114 +2996,411 @@
       <c r="F26" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K26" s="17">
+        <v>0.33</v>
+      </c>
+      <c r="L26" s="1">
+        <v>7</v>
+      </c>
+      <c r="M26" s="16">
+        <f t="shared" si="0"/>
+        <v>2.31</v>
+      </c>
+      <c r="N26" s="17">
+        <v>0.1178</v>
+      </c>
+      <c r="O26" s="9">
+        <f t="shared" si="2"/>
+        <v>0.8246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>18</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1623</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K27" s="17">
+        <v>4.95</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="16">
+        <f t="shared" si="0"/>
+        <v>4.95</v>
+      </c>
+      <c r="N27" s="17">
+        <v>4.95</v>
+      </c>
+      <c r="O27" s="9">
+        <f t="shared" si="2"/>
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>19</v>
+      </c>
       <c r="B28" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="H28" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K28" s="17">
+        <v>3.62</v>
+      </c>
+      <c r="L28" s="1">
+        <v>6</v>
+      </c>
+      <c r="M28" s="16">
+        <f t="shared" si="0"/>
+        <v>21.72</v>
+      </c>
+      <c r="N28" s="17">
+        <v>2.7458</v>
+      </c>
+      <c r="O28" s="9">
+        <f t="shared" si="2"/>
+        <v>16.474800000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>20</v>
+      </c>
       <c r="B29" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="H29" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K29" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1</v>
+      </c>
+      <c r="M29" s="16">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="N29" s="17">
+        <v>0.47670000000000001</v>
+      </c>
+      <c r="O29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.47670000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>21</v>
+      </c>
       <c r="B30" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="H30" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K30" s="17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1</v>
+      </c>
+      <c r="M30" s="16">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N30" s="17">
+        <v>0.44180000000000003</v>
+      </c>
+      <c r="O30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.44180000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>22</v>
+      </c>
       <c r="B31" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="D31" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K31" s="17">
+        <v>0.18</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
+      <c r="M31" s="16">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="N31" s="17">
+        <v>0.1036</v>
+      </c>
+      <c r="O31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.1036</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>23</v>
+      </c>
       <c r="B32" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K32" s="17">
+        <v>0.11</v>
+      </c>
+      <c r="L32" s="1">
+        <v>1</v>
+      </c>
+      <c r="M32" s="16">
+        <f t="shared" si="0"/>
+        <v>0.11</v>
+      </c>
+      <c r="N32" s="17">
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="O32" s="9">
+        <f t="shared" si="2"/>
+        <v>6.6500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>24</v>
+      </c>
       <c r="B33" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="K33" s="17">
+        <v>0.48</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+      <c r="M33" s="16">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="N33" s="17">
+        <v>0.31580000000000003</v>
+      </c>
+      <c r="O33" s="9">
+        <f t="shared" si="2"/>
+        <v>0.31580000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>25</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="K34" s="17">
+        <v>0.53</v>
+      </c>
+      <c r="L34" s="1">
+        <v>1</v>
+      </c>
+      <c r="M34" s="16">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+      <c r="N34" s="17">
+        <v>0.38129999999999997</v>
+      </c>
+      <c r="O34" s="9">
+        <f t="shared" si="2"/>
+        <v>0.38129999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>26</v>
+      </c>
       <c r="B35" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>60</v>
@@ -2271,44 +3411,95 @@
       <c r="H35" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
+      <c r="M35" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>27</v>
+      </c>
       <c r="B36" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" s="1">
+        <v>1</v>
+      </c>
+      <c r="M36" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>28</v>
+      </c>
       <c r="B37" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L37" s="1">
+        <v>1</v>
+      </c>
+      <c r="M37" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O37" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>29</v>
+      </c>
       <c r="B38" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>12</v>
@@ -2316,19 +3507,50 @@
       <c r="F38" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L38" s="1">
+        <v>1</v>
+      </c>
+      <c r="M38" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O38" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>30</v>
+      </c>
       <c r="B39" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1</v>
+      </c>
+      <c r="M39" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>